<commit_message>
commit changes to save
</commit_message>
<xml_diff>
--- a/src/schema/tools/controlledFromGooglesheet/ECRR Controlled Vocabularies.xlsx
+++ b/src/schema/tools/controlledFromGooglesheet/ECRR Controlled Vocabularies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\GithubC\earthcube\jsonld_forms\src\schema\tools\controlledFromGooglesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B82B326-A5F5-461E-A0E8-03A974A4475E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A774032-5729-4339-8BB1-096E9E0DE0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1725" yWindow="2355" windowWidth="26820" windowHeight="13620" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1695" yWindow="2400" windowWidth="26820" windowHeight="13620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Software Licenses" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,6 @@
     <definedName name="Usage">Usage!$A$2:$A$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -3113,7 +3112,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3386,6 +3385,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3999,7 +4002,9 @@
   </sheetPr>
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -4695,11 +4700,11 @@
         <v>654</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="15">
+    <row r="86" spans="1:2" ht="12.75">
       <c r="A86" s="77" t="s">
         <v>655</v>
       </c>
-      <c r="B86" s="78" t="s">
+      <c r="B86" s="106" t="s">
         <v>656</v>
       </c>
     </row>
@@ -5088,7 +5093,9 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -5121,7 +5128,7 @@
       <c r="A3" s="5" t="s">
         <v>707</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="97" t="s">
         <v>708</v>
       </c>
     </row>
@@ -5837,7 +5844,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="12.75">
+    <row r="23" spans="1:5" ht="15">
       <c r="A23" s="5" t="s">
         <v>836</v>
       </c>
@@ -42252,7 +42259,9 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -42367,6 +42376,7 @@
     <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -42377,8 +42387,8 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -42425,7 +42435,7 @@
       <c r="B3" s="57" t="s">
         <v>382</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="107" t="s">
         <v>383</v>
       </c>
       <c r="D3" s="103" t="s">

</xml_diff>